<commit_message>
Major helpers update, nearly all data functions coded.
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_RESInnovationCentreProject1-GridConstraints/Shared Documents/General/#. RN Offline Coding Zone/Curtailment-Analysis/testcases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="121_{C6FDF78E-BD6A-4C33-A22C-DAB90D031699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7FABA21-7F70-4F0B-907E-D1914B6DDF6E}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="121_{C6FDF78E-BD6A-4C33-A22C-DAB90D031699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E52FBEC1-E4B6-488B-A966-7648D1444DB3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -311,6 +311,18 @@
   </si>
   <si>
     <t>PGMINGEN</t>
+  </si>
+  <si>
+    <t>Bus 2, ABRO, Ca</t>
+  </si>
+  <si>
+    <t>Bus 1, Jack, Jen,        Carl</t>
+  </si>
+  <si>
+    <t>Gleeban</t>
+  </si>
+  <si>
+    <t>Gleyban</t>
   </si>
 </sst>
 </file>
@@ -4345,7 +4357,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4433,7 +4445,9 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="G2" s="10">
         <v>1</v>
       </c>
@@ -4476,7 +4490,9 @@
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="G3" s="10">
         <v>1</v>
       </c>
@@ -4610,7 +4626,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
@@ -4806,7 +4822,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -5009,26 +5025,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
     <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
@@ -5257,19 +5253,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CA13F78-96F4-4513-AAD3-BE41BCDA6AF8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5283,5 +5301,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CA13F78-96F4-4513-AAD3-BE41BCDA6AF8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
large helpers update, separating out filtering mechanic.
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="121_{C6FDF78E-BD6A-4C33-A22C-DAB90D031699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E52FBEC1-E4B6-488B-A966-7648D1444DB3}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="121_{C6FDF78E-BD6A-4C33-A22C-DAB90D031699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{142F8DE9-3779-4640-8020-F8F7762773A7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,9 +307,6 @@
     <t>t-12</t>
   </si>
   <si>
-    <t>Pro-Rata</t>
-  </si>
-  <si>
     <t>PGMINGEN</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Gleyban</t>
+  </si>
+  <si>
+    <t>LIFO</t>
   </si>
 </sst>
 </file>
@@ -4357,7 +4357,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4406,7 +4406,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>20</v>
@@ -4446,7 +4446,7 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
@@ -4491,7 +4491,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
@@ -4617,7 +4617,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -4626,7 +4626,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
@@ -4666,7 +4666,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
@@ -4715,7 +4715,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
@@ -4764,7 +4764,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
@@ -4813,7 +4813,7 @@
         <v>53</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D10" s="9">
         <v>2</v>
@@ -4822,7 +4822,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -4862,7 +4862,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D11" s="9">
         <v>2</v>
@@ -4911,7 +4911,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D12" s="9">
         <v>2</v>
@@ -4960,7 +4960,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D13" s="9">
         <v>2</v>
@@ -5014,7 +5014,7 @@
       <formula>($C2&lt;&gt;"Pro-Rata")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C13" xr:uid="{93378767-7322-405A-9798-43C52CE33CE3}">
       <formula1>"Individual,Uncontrollable,LIFO,Pro-Rata"</formula1>
     </dataValidation>
@@ -5025,6 +5025,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
     <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
@@ -5253,27 +5273,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CA13F78-96F4-4513-AAD3-BE41BCDA6AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5290,31 +5317,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
addition of objective, minor changes to defintiions.
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_RESInnovationCentreProject1-GridConstraints/Shared Documents/General/#. RN Offline Coding Zone/Curtailment-Analysis/testcases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="121_{C6FDF78E-BD6A-4C33-A22C-DAB90D031699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{142F8DE9-3779-4640-8020-F8F7762773A7}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="121_{C6FDF78E-BD6A-4C33-A22C-DAB90D031699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4B4AD23-3996-4603-9223-01725708DA1E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3180" yWindow="-13275" windowWidth="17280" windowHeight="9960" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="76">
   <si>
     <t>name</t>
   </si>
@@ -307,22 +307,10 @@
     <t>t-12</t>
   </si>
   <si>
+    <t>Pro-Rata</t>
+  </si>
+  <si>
     <t>PGMINGEN</t>
-  </si>
-  <si>
-    <t>Bus 2, ABRO, Ca</t>
-  </si>
-  <si>
-    <t>Bus 1, Jack, Jen,        Carl</t>
-  </si>
-  <si>
-    <t>Gleeban</t>
-  </si>
-  <si>
-    <t>Gleyban</t>
-  </si>
-  <si>
-    <t>LIFO</t>
   </si>
 </sst>
 </file>
@@ -4357,7 +4345,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4370,7 +4358,7 @@
     <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -4406,7 +4394,7 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>20</v>
@@ -4445,9 +4433,7 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="10" t="s">
-        <v>77</v>
-      </c>
+      <c r="F2" s="10"/>
       <c r="G2" s="10">
         <v>1</v>
       </c>
@@ -4490,9 +4476,7 @@
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="10" t="s">
-        <v>78</v>
-      </c>
+      <c r="F3" s="10"/>
       <c r="G3" s="10">
         <v>1</v>
       </c>
@@ -4617,7 +4601,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -4626,7 +4610,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
@@ -4666,7 +4650,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
@@ -4715,7 +4699,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
@@ -4764,7 +4748,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
@@ -4813,7 +4797,7 @@
         <v>53</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D10" s="9">
         <v>2</v>
@@ -4822,7 +4806,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -4862,7 +4846,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D11" s="9">
         <v>2</v>
@@ -4911,7 +4895,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D12" s="9">
         <v>2</v>
@@ -4960,7 +4944,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D13" s="9">
         <v>2</v>
@@ -5014,7 +4998,7 @@
       <formula>($C2&lt;&gt;"Pro-Rata")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C13" xr:uid="{93378767-7322-405A-9798-43C52CE33CE3}">
       <formula1>"Individual,Uncontrollable,LIFO,Pro-Rata"</formula1>
     </dataValidation>
@@ -5027,8 +5011,8 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+    <TaxCatchAll xmlns="23f97e4a-4cde-4203-a712-a632ca730d07" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b352a690-13b6-446a-ad80-20b9a9231a5f">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
@@ -5036,19 +5020,10 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
-    <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
-    <xsd:import namespace="3610aed6-0335-46d2-b190-87c476b048cc"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002AE3758F0CD35B4A92AADB38AC2CFEF2" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b74424f2ef32c27eb12382df101ff197">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b352a690-13b6-446a-ad80-20b9a9231a5f" xmlns:ns3="23f97e4a-4cde-4203-a712-a632ca730d07" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6340556347c2e6dcc1211b6bba07720" ns2:_="" ns3:_="">
+    <xsd:import namespace="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <xsd:import namespace="23f97e4a-4cde-4203-a712-a632ca730d07"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -5057,17 +5032,14 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5075,7 +5047,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6dce361f-7b53-4909-8b0d-30e42626cdc9" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b352a690-13b6-446a-ad80-20b9a9231a5f" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -5088,81 +5060,50 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="11" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="87865813-b24e-4515-aac3-72cd3b0aa1df" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="87865813-b24e-4515-aac3-72cd3b0aa1df" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3610aed6-0335-46d2-b190-87c476b048cc" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="23f97e4a-4cde-4203-a712-a632ca730d07" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{afb7282a-b4e1-44aa-9a85-3d59d972ca27}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="3610aed6-0335-46d2-b190-87c476b048cc">
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{709397c3-4097-4501-ae6f-3b9d11015068}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="23f97e4a-4cde-4203-a712-a632ca730d07">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -5273,6 +5214,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
   <ds:schemaRefs>
@@ -5286,29 +5236,19 @@
     <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CA13F78-96F4-4513-AAD3-BE41BCDA6AF8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8027663B-9396-462F-B5F0-B28574A9C9CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -5317,4 +5257,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated data_io to include timeseries data. Split obj_functions out of functions, functions renamed build_functions.
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -5011,8 +5011,8 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <TaxCatchAll xmlns="23f97e4a-4cde-4203-a712-a632ca730d07" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b352a690-13b6-446a-ad80-20b9a9231a5f">
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
@@ -5020,10 +5020,10 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002AE3758F0CD35B4A92AADB38AC2CFEF2" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b74424f2ef32c27eb12382df101ff197">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b352a690-13b6-446a-ad80-20b9a9231a5f" xmlns:ns3="23f97e4a-4cde-4203-a712-a632ca730d07" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6340556347c2e6dcc1211b6bba07720" ns2:_="" ns3:_="">
-    <xsd:import namespace="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <xsd:import namespace="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
+    <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <xsd:import namespace="3610aed6-0335-46d2-b190-87c476b048cc"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -5032,14 +5032,17 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5047,7 +5050,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b352a690-13b6-446a-ad80-20b9a9231a5f" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6dce361f-7b53-4909-8b0d-30e42626cdc9" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -5060,50 +5063,81 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="11" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="87865813-b24e-4515-aac3-72cd3b0aa1df" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="87865813-b24e-4515-aac3-72cd3b0aa1df" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="23f97e4a-4cde-4203-a712-a632ca730d07" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3610aed6-0335-46d2-b190-87c476b048cc" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{709397c3-4097-4501-ae6f-3b9d11015068}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="23f97e4a-4cde-4203-a712-a632ca730d07">
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{afb7282a-b4e1-44aa-9a85-3d59d972ca27}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="3610aed6-0335-46d2-b190-87c476b048cc">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -5241,22 +5275,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8027663B-9396-462F-B5F0-B28574A9C9CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19063C31-411A-4FED-97ED-8082117E9849}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Implementing all_island_iterations for timeseries analysis
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_RESInnovationCentreProject1-GridConstraints/Shared Documents/General/#. RN Offline Coding Zone/Curtailment-Analysis/testcases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="177" documentId="121_{C6FDF78E-BD6A-4C33-A22C-DAB90D031699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4B4AD23-3996-4603-9223-01725708DA1E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3180" yWindow="-13275" windowWidth="17280" windowHeight="9960" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -871,8 +871,8 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4344,7 +4344,7 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -5009,17 +5009,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
     <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
@@ -5248,6 +5237,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5258,6 +5258,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19063C31-411A-4FED-97ED-8082117E9849}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -5270,12 +5289,10 @@
     <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19063C31-411A-4FED-97ED-8082117E9849}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Added first version of extended RES model
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E91A6B29-52D4-442D-B1D6-A94D11FB6B9D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -461,6 +461,9 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,7 +874,7 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -3200,8 +3203,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4345,7 +4348,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4460,9 +4463,11 @@
         <v>400.68490000000003</v>
       </c>
       <c r="P2" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>200</v>
+      </c>
     </row>
     <row r="3" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
@@ -4503,9 +4508,11 @@
         <v>400.68490000000003</v>
       </c>
       <c r="P3" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>200</v>
+      </c>
     </row>
     <row r="4" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
@@ -4546,9 +4553,11 @@
         <v>400.68490000000003</v>
       </c>
       <c r="P4" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="Q4" s="22">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
@@ -4589,9 +4598,11 @@
         <v>400.68490000000003</v>
       </c>
       <c r="P5" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="Q5" s="22">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
@@ -4640,7 +4651,9 @@
       <c r="P6" s="13">
         <v>80</v>
       </c>
-      <c r="Q6" s="11"/>
+      <c r="Q6" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
@@ -4684,12 +4697,14 @@
         <v>0</v>
       </c>
       <c r="O7" s="10">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P7" s="13">
         <v>80</v>
       </c>
-      <c r="Q7" s="11"/>
+      <c r="Q7" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
@@ -4738,7 +4753,9 @@
       <c r="P8" s="13">
         <v>80</v>
       </c>
-      <c r="Q8" s="11"/>
+      <c r="Q8" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
@@ -4787,7 +4804,9 @@
       <c r="P9" s="13">
         <v>80</v>
       </c>
-      <c r="Q9" s="11"/>
+      <c r="Q9" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
@@ -4836,7 +4855,9 @@
       <c r="P10" s="13">
         <v>80</v>
       </c>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
@@ -4885,7 +4906,9 @@
       <c r="P11" s="13">
         <v>80</v>
       </c>
-      <c r="Q11" s="11"/>
+      <c r="Q11" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
@@ -4934,7 +4957,9 @@
       <c r="P12" s="13">
         <v>80</v>
       </c>
-      <c r="Q12" s="11"/>
+      <c r="Q12" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
@@ -4983,7 +5008,9 @@
       <c r="P13" s="13">
         <v>80</v>
       </c>
-      <c r="Q13" s="11"/>
+      <c r="Q13" s="22">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q9" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
@@ -5009,6 +5036,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100206C8747921DEB47908282AF5FC82B21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd288e11850d22ee40981664a927e65e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6dce361f-7b53-4909-8b0d-30e42626cdc9" xmlns:ns3="3610aed6-0335-46d2-b190-87c476b048cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8a8939e80faa41470004db56e4a3333" ns2:_="" ns3:_="">
     <xsd:import namespace="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
@@ -5237,17 +5275,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5258,6 +5285,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19063C31-411A-4FED-97ED-8082117E9849}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5276,25 +5322,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
secure copperplate optimisation formulation added.
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E91A6B29-52D4-442D-B1D6-A94D11FB6B9D}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCC9575-1173-46D1-8606-2681623658C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">branch!$A$1:$I$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">generator!$A$1:$Q$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">generator!$A$1:$R$9</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">ts_PD!$F$16:$G$16</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="82">
   <si>
     <t>name</t>
   </si>
@@ -311,6 +311,24 @@
   </si>
   <si>
     <t>PGMINGEN</t>
+  </si>
+  <si>
+    <t>MUON_group</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>S_NBMIN_DUB_L2, S_REP_ROI</t>
+  </si>
+  <si>
+    <t>S_NBMIN_MP_NB, S_REP_ROI</t>
+  </si>
+  <si>
+    <t>S_NBMIN_CPS, S_MWMAX_NI_GT</t>
   </si>
 </sst>
 </file>
@@ -403,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -464,6 +482,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,7 +818,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,8 +850,8 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
+      <c r="D2" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -843,8 +864,8 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
+      <c r="D3" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -857,8 +878,8 @@
       <c r="C4" s="3">
         <v>3</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
+      <c r="D4" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1426,7 +1447,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G13"/>
+      <selection activeCell="D21" sqref="D21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,16 +1498,16 @@
         <v>62</v>
       </c>
       <c r="B2" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D2" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E2" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F2" s="9">
         <v>0</v>
@@ -1518,16 +1539,16 @@
         <v>63</v>
       </c>
       <c r="B3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C3" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D3" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E3" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F3" s="9">
         <v>0</v>
@@ -1559,16 +1580,16 @@
         <v>64</v>
       </c>
       <c r="B4" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C4" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D4" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F4" s="9">
         <v>0</v>
@@ -1600,16 +1621,16 @@
         <v>65</v>
       </c>
       <c r="B5" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F5" s="9">
         <v>0</v>
@@ -1641,16 +1662,16 @@
         <v>66</v>
       </c>
       <c r="B6" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C6" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D6" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E6" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F6" s="9">
         <v>0</v>
@@ -1682,16 +1703,16 @@
         <v>67</v>
       </c>
       <c r="B7" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C7" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D7" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E7" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9">
         <v>0</v>
@@ -1723,16 +1744,16 @@
         <v>68</v>
       </c>
       <c r="B8" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C8" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D8" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E8" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F8" s="9">
         <v>0</v>
@@ -1764,16 +1785,16 @@
         <v>69</v>
       </c>
       <c r="B9" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C9" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D9" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E9" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F9" s="9">
         <v>0</v>
@@ -1805,16 +1826,16 @@
         <v>70</v>
       </c>
       <c r="B10" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C10" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D10" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E10" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F10" s="9">
         <v>0</v>
@@ -1846,16 +1867,16 @@
         <v>71</v>
       </c>
       <c r="B11" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D11" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E11" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F11" s="9">
         <v>0</v>
@@ -1887,16 +1908,16 @@
         <v>72</v>
       </c>
       <c r="B12" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C12" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E12" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F12" s="9">
         <v>0</v>
@@ -1928,16 +1949,16 @@
         <v>73</v>
       </c>
       <c r="B13" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C13" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D13" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E13" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F13" s="9">
         <v>0</v>
@@ -1977,7 +1998,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3203,8 +3224,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3299,8 +3320,8 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3329,7 +3350,7 @@
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="23">
         <f>(60-40)*0.5*SIN((PI())/6*COUNTA($A$2:$A2)-PI()/2)+(60+40)*0.5</f>
         <v>41.339745962155611</v>
       </c>
@@ -4345,10 +4366,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4359,19 +4380,20 @@
     <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="1017" width="8.44140625" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="1018" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4391,40 +4413,43 @@
         <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -4437,39 +4462,42 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="10">
+      <c r="G2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="10">
         <v>1</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12">
-        <v>0</v>
-      </c>
+      <c r="I2" s="11"/>
       <c r="J2" s="12">
-        <v>2</v>
-      </c>
-      <c r="K2" s="21">
+        <v>0</v>
+      </c>
+      <c r="K2" s="12">
+        <v>10</v>
+      </c>
+      <c r="L2" s="21">
         <v>50</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="10">
+      <c r="O2" s="10">
         <v>129</v>
       </c>
-      <c r="O2" s="15">
+      <c r="P2" s="15">
         <v>400.68490000000003</v>
       </c>
-      <c r="P2" s="13">
+      <c r="Q2" s="13">
         <v>90</v>
       </c>
-      <c r="Q2" s="22">
+      <c r="R2" s="22">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -4482,39 +4510,42 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="10">
+      <c r="G3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="10">
         <v>1</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12">
+      <c r="I3" s="11"/>
+      <c r="J3" s="12">
         <v>10</v>
       </c>
-      <c r="J3" s="12">
-        <v>2</v>
-      </c>
-      <c r="K3" s="21">
+      <c r="K3" s="12">
+        <v>20</v>
+      </c>
+      <c r="L3" s="21">
         <v>100</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="10">
+      <c r="O3" s="10">
         <v>130</v>
       </c>
-      <c r="O3" s="15">
+      <c r="P3" s="15">
         <v>400.68490000000003</v>
       </c>
-      <c r="P3" s="13">
+      <c r="Q3" s="13">
         <v>90</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="R3" s="22">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -4527,39 +4558,42 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="10">
+      <c r="G4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="10">
         <v>1</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12">
+      <c r="I4" s="11"/>
+      <c r="J4" s="12">
         <v>10</v>
       </c>
-      <c r="J4" s="12">
-        <v>2</v>
-      </c>
-      <c r="K4" s="21">
+      <c r="K4" s="12">
+        <v>20</v>
+      </c>
+      <c r="L4" s="21">
         <v>100</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="10">
+      <c r="O4" s="10">
         <v>130</v>
       </c>
-      <c r="O4" s="15">
+      <c r="P4" s="15">
         <v>400.68490000000003</v>
       </c>
-      <c r="P4" s="13">
+      <c r="Q4" s="13">
         <v>90</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="R4" s="22">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -4572,39 +4606,42 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="10">
+      <c r="G5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="10">
         <v>1</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12">
-        <v>0</v>
-      </c>
+      <c r="I5" s="11"/>
       <c r="J5" s="12">
-        <v>2</v>
-      </c>
-      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>40</v>
+      </c>
+      <c r="L5" s="21">
         <v>200</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="10">
+      <c r="O5" s="10">
         <v>130</v>
       </c>
-      <c r="O5" s="15">
+      <c r="P5" s="15">
         <v>400.68490000000003</v>
       </c>
-      <c r="P5" s="13">
+      <c r="Q5" s="13">
         <v>90</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="R5" s="22">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -4623,39 +4660,40 @@
       <c r="F6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12">
-        <v>0</v>
-      </c>
+      <c r="I6" s="11"/>
       <c r="J6" s="12">
         <v>0</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
         <v>24.453486016540655</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="10">
-        <v>0</v>
-      </c>
       <c r="O6" s="10">
         <v>0</v>
       </c>
-      <c r="P6" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q6" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R6" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>1</v>
       </c>
@@ -4674,39 +4712,40 @@
       <c r="F7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10">
         <v>1</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
+      <c r="I7" s="11"/>
       <c r="J7" s="12">
         <v>0</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="12">
+        <v>0</v>
+      </c>
+      <c r="L7" s="20">
         <v>36.402073474160886</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="N7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="10">
-        <v>0</v>
-      </c>
       <c r="O7" s="10">
-        <v>10000</v>
-      </c>
-      <c r="P7" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q7" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R7" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -4725,39 +4764,40 @@
       <c r="F8" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
         <v>1</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12">
-        <v>0</v>
-      </c>
+      <c r="I8" s="11"/>
       <c r="J8" s="12">
         <v>0</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="20">
         <v>29.550761662855376</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="N8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="10">
-        <v>0</v>
-      </c>
       <c r="O8" s="10">
         <v>0</v>
       </c>
-      <c r="P8" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R8" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>1</v>
       </c>
@@ -4776,39 +4816,40 @@
       <c r="F9" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
         <v>1</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12">
-        <v>0</v>
-      </c>
+      <c r="I9" s="11"/>
       <c r="J9" s="12">
         <v>0</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="12">
+        <v>0</v>
+      </c>
+      <c r="L9" s="20">
         <v>29.175813615177187</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="N9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="10">
-        <v>0</v>
-      </c>
       <c r="O9" s="10">
         <v>0</v>
       </c>
-      <c r="P9" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R9" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -4827,39 +4868,40 @@
       <c r="F10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10">
         <v>1</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12">
-        <v>0</v>
-      </c>
+      <c r="I10" s="11"/>
       <c r="J10" s="12">
         <v>0</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="20">
         <v>8.00751150094829</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="N10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="10">
-        <v>0</v>
-      </c>
       <c r="O10" s="10">
         <v>0</v>
       </c>
-      <c r="P10" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q10" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R10" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>2</v>
       </c>
@@ -4878,39 +4920,40 @@
       <c r="F11" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10">
         <v>1</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12">
-        <v>0</v>
-      </c>
+      <c r="I11" s="11"/>
       <c r="J11" s="12">
         <v>0</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="12">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20">
         <v>6.7648700785818461</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="M11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="N11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N11" s="10">
-        <v>0</v>
-      </c>
       <c r="O11" s="10">
         <v>0</v>
       </c>
-      <c r="P11" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R11" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>2</v>
       </c>
@@ -4929,39 +4972,40 @@
       <c r="F12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10">
         <v>1</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12">
-        <v>0</v>
-      </c>
+      <c r="I12" s="11"/>
       <c r="J12" s="12">
         <v>0</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="20">
         <v>9.545660845922793</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="M12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="N12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="10">
-        <v>0</v>
-      </c>
       <c r="O12" s="10">
         <v>0</v>
       </c>
-      <c r="P12" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R12" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>2</v>
       </c>
@@ -4980,40 +5024,41 @@
       <c r="F13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10">
         <v>1</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12">
-        <v>0</v>
-      </c>
+      <c r="I13" s="11"/>
       <c r="J13" s="12">
         <v>0</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="12">
+        <v>0</v>
+      </c>
+      <c r="L13" s="20">
         <v>5.224351111058203</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="M13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="N13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="10">
-        <v>0</v>
-      </c>
       <c r="O13" s="10">
         <v>0</v>
       </c>
-      <c r="P13" s="13">
-        <v>80</v>
-      </c>
-      <c r="Q13" s="22">
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>-20</v>
+      </c>
+      <c r="R13" s="22">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q9" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
+  <autoFilter ref="A1:R9" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="D2:E13">
     <cfRule type="expression" dxfId="1" priority="3">
@@ -5036,14 +5081,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5276,29 +5319,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5323,9 +5357,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Incorrect assignment of M_LB and M_UB in big-M constraints fixed.
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="81" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCC9575-1173-46D1-8606-2681623658C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -3320,8 +3320,8 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4368,8 +4368,8 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5081,12 +5081,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5319,20 +5321,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5357,20 +5368,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DCOPF model formulation completed
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCC9575-1173-46D1-8606-2681623658C6}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37C61349-DF8F-447F-8D60-C7436F933F06}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>S_NBMIN_CPS, S_MWMAX_NI_GT</t>
+  </si>
+  <si>
+    <t>Bus 1, Combo</t>
+  </si>
+  <si>
+    <t>Bus 2, Combo</t>
   </si>
 </sst>
 </file>
@@ -4369,7 +4375,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4814,7 +4820,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10">
@@ -4866,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10">
@@ -5081,14 +5087,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5321,29 +5325,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5368,9 +5363,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added data to excel output
</commit_message>
<xml_diff>
--- a/end-to-end-testcase.xlsx
+++ b/end-to-end-testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath.sharepoint.com/sites/EEE_STU_NayerPhD/Shared Documents/General/18. RES Research PSCC 2026 Paper/oats_curtailment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37C61349-DF8F-447F-8D60-C7436F933F06}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="114_{D301639E-74A8-4237-8286-F30DBF25EDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2D8725A-6DE2-4F39-A4B8-85DB1D4204CC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4375,7 +4375,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R6" s="22">
         <v>0</v>
@@ -4745,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R7" s="22">
         <v>0</v>
@@ -4797,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R8" s="22">
         <v>0</v>
@@ -4849,7 +4849,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R9" s="22">
         <v>0</v>
@@ -4901,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R10" s="22">
         <v>0</v>
@@ -4953,7 +4953,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R11" s="22">
         <v>0</v>
@@ -5005,7 +5005,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R12" s="22">
         <v>0</v>
@@ -5057,7 +5057,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="13">
-        <v>-20</v>
+        <v>1000</v>
       </c>
       <c r="R13" s="22">
         <v>0</v>
@@ -5087,12 +5087,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5325,20 +5327,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3610aed6-0335-46d2-b190-87c476b048cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6dce361f-7b53-4909-8b0d-30e42626cdc9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
+    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
+    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5363,20 +5374,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C8DCC68-DE29-405F-AF91-B4AEFE460474}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE53B3-CBA2-4721-BCB6-3D852AD2B7E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23f97e4a-4cde-4203-a712-a632ca730d07"/>
-    <ds:schemaRef ds:uri="b352a690-13b6-446a-ad80-20b9a9231a5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3610aed6-0335-46d2-b190-87c476b048cc"/>
-    <ds:schemaRef ds:uri="6dce361f-7b53-4909-8b0d-30e42626cdc9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>